<commit_message>
prices updated, zod validation for cabinets added
</commit_message>
<xml_diff>
--- a/backend/data/database.xlsx
+++ b/backend/data/database.xlsx
@@ -8,24 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\ledts\calculator\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900C2FA7-A769-4089-8300-AE20A465274E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722153BC-72B0-48E4-85E5-5B910F111784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15600" yWindow="0" windowWidth="36000" windowHeight="20880" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScreenTypes" sheetId="1" r:id="rId1"/>
     <sheet name="PixelSteps" sheetId="2" r:id="rId2"/>
     <sheet name="Cabinets" sheetId="3" r:id="rId3"/>
     <sheet name="IngressProtection" sheetId="4" r:id="rId4"/>
-    <sheet name="PartsPriceUsd" sheetId="6" r:id="rId5"/>
-    <sheet name="PartsPriceRub" sheetId="5" r:id="rId6"/>
+    <sheet name="PartsPrice" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="245">
   <si>
     <t>name</t>
   </si>
@@ -276,12 +275,6 @@
     <t>P4, P4 Pro, P3.07, P3.07 Pro, P2.5, P2.5 Pro, P2, P1.86, P1.86 Pro</t>
   </si>
   <si>
-    <t>480*640_C AL фронтальный интерьерный шаг пикселя до 1.86</t>
-  </si>
-  <si>
-    <t>480*640_C AL фронтальный интерьерный шаг пикселя ниже 1.86</t>
-  </si>
-  <si>
     <t>P1.66 Pro, P1.53 Pro, P1.37 Pro, P1.25 Pro</t>
   </si>
   <si>
@@ -576,18 +569,6 @@
     <t>БП200</t>
   </si>
   <si>
-    <t>detail</t>
-  </si>
-  <si>
-    <t>priceUSD</t>
-  </si>
-  <si>
-    <t>priceRUB</t>
-  </si>
-  <si>
-    <t>detailEn</t>
-  </si>
-  <si>
     <t>PU200</t>
   </si>
   <si>
@@ -766,6 +747,18 @@
   </si>
   <si>
     <t>flexibleScreen</t>
+  </si>
+  <si>
+    <t>640*480_C AL фронтальный интерьерный шаг пикселя до 1.86</t>
+  </si>
+  <si>
+    <t>640*480_C AL фронтальный интерьерный шаг пикселя ниже 1.86</t>
+  </si>
+  <si>
+    <t>nameEn</t>
+  </si>
+  <si>
+    <t>priceRub</t>
   </si>
 </sst>
 </file>
@@ -2146,8 +2139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2181,7 +2174,7 @@
         <v>48</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>50</v>
@@ -2234,7 +2227,7 @@
         <v>18</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F2" s="2">
         <v>300</v>
@@ -2287,7 +2280,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F3" s="2">
         <v>200</v>
@@ -2340,7 +2333,7 @@
         <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F4" s="2">
         <v>200</v>
@@ -2393,7 +2386,7 @@
         <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F5" s="2">
         <v>200</v>
@@ -2446,7 +2439,7 @@
         <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F6" s="2">
         <v>200</v>
@@ -2499,7 +2492,7 @@
         <v>9</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F7" s="2">
         <v>200</v>
@@ -2552,7 +2545,7 @@
         <v>4</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F8" s="2">
         <v>200</v>
@@ -2605,7 +2598,7 @@
         <v>4</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F9" s="2">
         <v>200</v>
@@ -2658,7 +2651,7 @@
         <v>4</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F10" s="2">
         <v>200</v>
@@ -2711,7 +2704,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F11" s="2">
         <v>300</v>
@@ -2764,7 +2757,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F12" s="2">
         <v>200</v>
@@ -2817,7 +2810,7 @@
         <v>8</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F13" s="2">
         <v>200</v>
@@ -2870,7 +2863,7 @@
         <v>8</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F14" s="2">
         <v>200</v>
@@ -2911,19 +2904,19 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>83</v>
+        <v>241</v>
       </c>
       <c r="B15" s="1">
+        <v>640</v>
+      </c>
+      <c r="C15" s="1">
         <v>480</v>
-      </c>
-      <c r="C15" s="1">
-        <v>640</v>
       </c>
       <c r="D15" s="2">
         <v>6</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F15" s="2">
         <v>200</v>
@@ -2964,19 +2957,19 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>84</v>
+        <v>242</v>
       </c>
       <c r="B16" s="1">
+        <v>640</v>
+      </c>
+      <c r="C16" s="1">
         <v>480</v>
-      </c>
-      <c r="C16" s="1">
-        <v>640</v>
       </c>
       <c r="D16" s="2">
         <v>6</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F16" s="2">
         <v>300</v>
@@ -2991,7 +2984,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>6</v>
@@ -3043,783 +3036,783 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>89</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -3834,10 +3827,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C85276AB-6D20-4E24-BA3A-1994BA2758AE}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3848,24 +3841,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>183</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>186</v>
+        <v>243</v>
       </c>
       <c r="C1" t="s">
-        <v>184</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>185</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B2" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C2">
         <v>9</v>
@@ -3873,10 +3866,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C3">
         <v>16</v>
@@ -3884,7 +3877,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
@@ -3895,10 +3888,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B5" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C5">
         <v>20</v>
@@ -3906,7 +3899,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B6" t="s">
         <v>52</v>
@@ -3917,10 +3910,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B7" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -3928,10 +3921,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B8" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C8">
         <v>6.5</v>
@@ -3939,10 +3932,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B9" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C9">
         <v>8.5</v>
@@ -3950,10 +3943,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B10" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C10">
         <v>8.5</v>
@@ -3961,10 +3954,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B11" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C11">
         <v>8.5</v>
@@ -3972,266 +3965,232 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B12" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C12">
         <v>8.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>187</v>
+      </c>
+      <c r="B13" t="s">
+        <v>235</v>
+      </c>
+      <c r="D13">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>188</v>
+      </c>
+      <c r="B14" t="s">
+        <v>213</v>
+      </c>
+      <c r="D14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>189</v>
+      </c>
+      <c r="B15" t="s">
+        <v>214</v>
+      </c>
+      <c r="D15">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>190</v>
+      </c>
+      <c r="B16" t="s">
+        <v>215</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>191</v>
+      </c>
+      <c r="B17" t="s">
+        <v>216</v>
+      </c>
+      <c r="D17">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>192</v>
+      </c>
+      <c r="B18" t="s">
+        <v>217</v>
+      </c>
+      <c r="D18">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>193</v>
+      </c>
+      <c r="B19" t="s">
+        <v>218</v>
+      </c>
+      <c r="D19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>199</v>
+      </c>
+      <c r="B20" t="s">
+        <v>233</v>
+      </c>
+      <c r="D20">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>200</v>
+      </c>
+      <c r="B21" t="s">
+        <v>224</v>
+      </c>
+      <c r="D21">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>201</v>
+      </c>
+      <c r="B22" t="s">
+        <v>225</v>
+      </c>
+      <c r="D22">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>226</v>
+      </c>
+      <c r="B23" t="s">
+        <v>227</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>202</v>
+      </c>
+      <c r="B24" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>203</v>
+      </c>
+      <c r="B25" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>204</v>
+      </c>
+      <c r="B26" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>205</v>
+      </c>
+      <c r="B27" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>206</v>
+      </c>
+      <c r="B28" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>207</v>
+      </c>
+      <c r="B29" t="s">
+        <v>236</v>
+      </c>
+      <c r="D29">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>208</v>
+      </c>
+      <c r="B30" t="s">
+        <v>237</v>
+      </c>
+      <c r="D30">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>209</v>
+      </c>
+      <c r="B31" t="s">
+        <v>238</v>
+      </c>
+      <c r="D31">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>210</v>
+      </c>
+      <c r="B32" t="s">
+        <v>239</v>
+      </c>
+      <c r="D32">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>211</v>
+      </c>
+      <c r="B33" t="s">
+        <v>240</v>
+      </c>
+      <c r="D33">
+        <v>15000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE23C598-F713-4636-BBE4-4C6254A2B82A}">
-  <dimension ref="A1:D22"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="17" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B2" t="s">
-        <v>241</v>
-      </c>
-      <c r="D2">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B3" t="s">
-        <v>219</v>
-      </c>
-      <c r="D3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>195</v>
-      </c>
-      <c r="B4" t="s">
-        <v>220</v>
-      </c>
-      <c r="D4">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>196</v>
-      </c>
-      <c r="B5" t="s">
-        <v>221</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>197</v>
-      </c>
-      <c r="B6" t="s">
-        <v>222</v>
-      </c>
-      <c r="D6">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>198</v>
-      </c>
-      <c r="B7" t="s">
-        <v>223</v>
-      </c>
-      <c r="D7">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>199</v>
-      </c>
-      <c r="B8" t="s">
-        <v>224</v>
-      </c>
-      <c r="D8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>205</v>
-      </c>
-      <c r="B9" t="s">
-        <v>239</v>
-      </c>
-      <c r="D9">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>206</v>
-      </c>
-      <c r="B10" t="s">
-        <v>230</v>
-      </c>
-      <c r="D10">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>207</v>
-      </c>
-      <c r="B11" t="s">
-        <v>231</v>
-      </c>
-      <c r="D11">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>232</v>
-      </c>
-      <c r="B12" t="s">
-        <v>233</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>208</v>
-      </c>
-      <c r="B13" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>209</v>
-      </c>
-      <c r="B14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>210</v>
-      </c>
-      <c r="B15" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>211</v>
-      </c>
-      <c r="B16" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>212</v>
-      </c>
-      <c r="B17" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>213</v>
-      </c>
-      <c r="B18" t="s">
-        <v>242</v>
-      </c>
-      <c r="D18">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>214</v>
-      </c>
-      <c r="B19" t="s">
-        <v>243</v>
-      </c>
-      <c r="D19">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>215</v>
-      </c>
-      <c r="B20" t="s">
-        <v>244</v>
-      </c>
-      <c r="D20">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>216</v>
-      </c>
-      <c r="B21" t="s">
-        <v>245</v>
-      </c>
-      <c r="D21">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>217</v>
-      </c>
-      <c r="B22" t="s">
-        <v>246</v>
-      </c>
-      <c r="D22">
-        <v>15000</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated with Pitch filtration logic
</commit_message>
<xml_diff>
--- a/backend/data/database.xlsx
+++ b/backend/data/database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\ledts\calculator\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8D9E57-4E4E-459C-ABAE-8B164CD89ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBC8486-74EB-467A-934B-F58508694267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25590" yWindow="0" windowWidth="26010" windowHeight="20880" tabRatio="1000" firstSheet="27" activeTab="34" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="1000" firstSheet="32" activeTab="39" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="screen_type" sheetId="22" r:id="rId1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2675" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2610" uniqueCount="558">
   <si>
     <t>уличный</t>
   </si>
@@ -1744,17 +1744,54 @@
   <si>
     <t>160x160</t>
   </si>
+  <si>
+    <t>LC-CA-576575</t>
+  </si>
+  <si>
+    <t>Кабинет стальной задний уличный</t>
+  </si>
+  <si>
+    <t>Кабинет стальной фронтальный уличный</t>
+  </si>
+  <si>
+    <t>Кабинет стальной задний интерьерный</t>
+  </si>
+  <si>
+    <t>Кабинет стальной фронтальный интерьерный</t>
+  </si>
+  <si>
+    <t>NN-CSRO</t>
+  </si>
+  <si>
+    <t>NN-CSFO</t>
+  </si>
+  <si>
+    <t>NN-CSRI</t>
+  </si>
+  <si>
+    <t>NN-CSFI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P2 </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1818,21 +1855,22 @@
       <charset val="204"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
-      <name val="Arial"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1842,6 +1880,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1855,94 +1899,154 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{5033A922-AEBE-4CDD-9FD8-03B9F0448B35}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{A577549E-2D2E-4165-A7C2-32844398B967}"/>
     <cellStyle name="Normal 4" xfId="3" xr:uid="{C64E5450-0B80-4AD3-8FC7-937A00180176}"/>
+    <cellStyle name="Normal 5" xfId="4" xr:uid="{ED67CD53-254C-476B-A43A-A6D366E9B16E}"/>
   </cellStyles>
-  <dxfs count="53">
+  <dxfs count="57">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2696,10 +2800,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>513</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>183</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -2885,7 +2989,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="44" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2962,7 +3066,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="43" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3994,7 +4098,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D2">
-    <cfRule type="duplicateValues" dxfId="42" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4523,9 +4627,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A2:D45" xr:uid="{D1557351-AC75-4275-84AC-10988B807ED9}"/>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A2:B2">
-    <cfRule type="duplicateValues" dxfId="41" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4582,16 +4686,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="27">
+      <c r="A3" s="26">
         <v>320160</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>370</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="26">
         <v>320</v>
       </c>
-      <c r="D3" s="27">
+      <c r="D3" s="26">
         <v>160</v>
       </c>
       <c r="E3" s="6" t="s">
@@ -4599,16 +4703,16 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="27">
+      <c r="A4" s="26">
         <v>192192</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="26" t="s">
         <v>408</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="26">
         <v>192</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="26">
         <v>192</v>
       </c>
       <c r="E4" s="6" t="s">
@@ -4616,16 +4720,16 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="27">
+      <c r="A5" s="26">
         <v>250250</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>420</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="26">
         <v>250</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="26">
         <v>250</v>
       </c>
       <c r="E5" s="6" t="s">
@@ -4633,16 +4737,16 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="27">
+      <c r="A6" s="26">
         <v>240120</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="26" t="s">
         <v>421</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="26">
         <v>240</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="26">
         <v>120</v>
       </c>
       <c r="E6" s="6" t="s">
@@ -4650,7 +4754,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="27">
+      <c r="A7" s="26">
         <v>256128</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -4702,7 +4806,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E2">
-    <cfRule type="duplicateValues" dxfId="40" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4710,16 +4814,15 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A087147-0889-47E2-B7E5-6733E2DA4BB8}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D29"/>
+      <selection activeCell="A30" sqref="A30:A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="16" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="16" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="72.85546875" style="6" customWidth="1"/>
     <col min="4" max="4" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
@@ -4754,7 +4857,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="30" t="s">
         <v>306</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -4763,12 +4866,12 @@
       <c r="C3" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="D3" s="19" t="s">
-        <v>409</v>
+      <c r="D3" s="1" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="30" t="s">
         <v>307</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -4777,12 +4880,12 @@
       <c r="C4" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="D4" s="19" t="s">
-        <v>409</v>
+      <c r="D4" s="1" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="30" t="s">
         <v>308</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -4791,8 +4894,8 @@
       <c r="C5" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="D5" s="19" t="s">
-        <v>409</v>
+      <c r="D5" s="1" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4819,8 +4922,8 @@
       <c r="C7" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="D7" s="19" t="s">
-        <v>409</v>
+      <c r="D7" s="1" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -4833,8 +4936,8 @@
       <c r="C8" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="D8" s="19" t="s">
-        <v>409</v>
+      <c r="D8" s="1" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -4847,8 +4950,8 @@
       <c r="C9" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="D9" s="19" t="s">
-        <v>409</v>
+      <c r="D9" s="1" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4861,8 +4964,8 @@
       <c r="C10" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="D10" s="19" t="s">
-        <v>409</v>
+      <c r="D10" s="1" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -4875,8 +4978,8 @@
       <c r="C11" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="D11" s="19" t="s">
-        <v>409</v>
+      <c r="D11" s="1" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -4889,8 +4992,8 @@
       <c r="C12" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="D12" s="19" t="s">
-        <v>409</v>
+      <c r="D12" s="1" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -4904,7 +5007,7 @@
         <v>391</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -4918,7 +5021,7 @@
         <v>392</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -4932,7 +5035,7 @@
         <v>393</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -4946,7 +5049,7 @@
         <v>394</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -4960,7 +5063,7 @@
         <v>395</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -4974,7 +5077,7 @@
         <v>396</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -4988,7 +5091,7 @@
         <v>397</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -5002,7 +5105,7 @@
         <v>398</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -5016,7 +5119,7 @@
         <v>406</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -5030,7 +5133,7 @@
         <v>407</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -5044,7 +5147,7 @@
         <v>404</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -5058,7 +5161,7 @@
         <v>399</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -5072,7 +5175,7 @@
         <v>405</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -5086,7 +5189,7 @@
         <v>400</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -5100,7 +5203,7 @@
         <v>401</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -5114,7 +5217,7 @@
         <v>402</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -5128,23 +5231,82 @@
         <v>403</v>
       </c>
       <c r="D29" s="19" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
+        <v>554</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>554</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>550</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>551</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>556</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>556</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>552</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>411</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:C12" xr:uid="{3A087147-0889-47E2-B7E5-6733E2DA4BB8}"/>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="39" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:A29">
-    <cfRule type="duplicateValues" dxfId="38" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="37" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C2">
-    <cfRule type="duplicateValues" dxfId="36" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30:A33">
+    <cfRule type="duplicateValues" dxfId="39" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5155,7 +5317,7 @@
   <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5166,7 +5328,7 @@
     <col min="4" max="4" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9.140625" style="6"/>
-    <col min="8" max="8" width="9.140625" style="30"/>
+    <col min="8" max="8" width="9.140625" style="29"/>
     <col min="9" max="15" width="9.140625" style="6"/>
     <col min="16" max="16" width="15.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
@@ -5210,10 +5372,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="29">
+      <c r="A2" s="28">
         <v>320160</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
         <v>370</v>
       </c>
       <c r="C2" s="6">
@@ -5243,10 +5405,10 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" s="29">
+      <c r="A3" s="28">
         <v>480480</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="28" t="s">
         <v>372</v>
       </c>
       <c r="C3" s="6">
@@ -5276,10 +5438,10 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" s="29">
+      <c r="A4" s="28">
         <v>5001000</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="28" t="s">
         <v>365</v>
       </c>
       <c r="C4" s="6">
@@ -5309,10 +5471,10 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="29">
+      <c r="A5" s="28">
         <v>500500</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="28" t="s">
         <v>364</v>
       </c>
       <c r="C5" s="6">
@@ -5342,10 +5504,10 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="29">
+      <c r="A6" s="28">
         <v>512512</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="28" t="s">
         <v>366</v>
       </c>
       <c r="C6" s="6">
@@ -5375,10 +5537,10 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A7" s="29">
+      <c r="A7" s="28">
         <v>576576</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="28" t="s">
         <v>367</v>
       </c>
       <c r="C7" s="6">
@@ -5408,10 +5570,10 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A8" s="29">
+      <c r="A8" s="28">
         <v>640480</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="28" t="s">
         <v>369</v>
       </c>
       <c r="C8" s="6">
@@ -5441,10 +5603,10 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A9" s="29">
+      <c r="A9" s="28">
         <v>640576</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="28" t="s">
         <v>368</v>
       </c>
       <c r="C9" s="6">
@@ -5474,10 +5636,10 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A10" s="29">
+      <c r="A10" s="28">
         <v>640640</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="28" t="s">
         <v>363</v>
       </c>
       <c r="C10" s="6">
@@ -5507,10 +5669,10 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A11" s="29">
+      <c r="A11" s="28">
         <v>9601120</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="28" t="s">
         <v>373</v>
       </c>
       <c r="C11" s="6">
@@ -5540,10 +5702,10 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A12" s="29">
+      <c r="A12" s="28">
         <v>960960</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="28" t="s">
         <v>371</v>
       </c>
       <c r="C12" s="6">
@@ -5590,120 +5752,130 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="P14" s="30"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="30"/>
-      <c r="S14" s="30"/>
-      <c r="T14" s="30"/>
+      <c r="P14" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="29">
+        <v>0</v>
+      </c>
+      <c r="R14" s="29">
+        <v>0</v>
+      </c>
+      <c r="S14" s="29">
+        <v>0</v>
+      </c>
+      <c r="T14" s="6" t="s">
+        <v>411</v>
+      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="P15" s="30"/>
-      <c r="Q15" s="30"/>
-      <c r="R15" s="30"/>
-      <c r="S15" s="30"/>
-      <c r="T15" s="30"/>
+      <c r="P15" s="29"/>
+      <c r="Q15" s="29"/>
+      <c r="R15" s="29"/>
+      <c r="S15" s="29"/>
+      <c r="T15" s="29"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="P16" s="30"/>
-      <c r="Q16" s="30"/>
-      <c r="R16" s="30"/>
-      <c r="S16" s="30"/>
-      <c r="T16" s="30"/>
+      <c r="P16" s="29"/>
+      <c r="Q16" s="29"/>
+      <c r="R16" s="29"/>
+      <c r="S16" s="29"/>
+      <c r="T16" s="29"/>
     </row>
     <row r="17" spans="16:20" x14ac:dyDescent="0.2">
-      <c r="P17" s="30"/>
-      <c r="Q17" s="30"/>
-      <c r="R17" s="30"/>
-      <c r="S17" s="30"/>
-      <c r="T17" s="30"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="29"/>
+      <c r="R17" s="29"/>
+      <c r="S17" s="29"/>
+      <c r="T17" s="29"/>
     </row>
     <row r="18" spans="16:20" x14ac:dyDescent="0.2">
-      <c r="P18" s="30"/>
-      <c r="Q18" s="30"/>
-      <c r="R18" s="30"/>
-      <c r="S18" s="30"/>
-      <c r="T18" s="30"/>
+      <c r="P18" s="29"/>
+      <c r="Q18" s="29"/>
+      <c r="R18" s="29"/>
+      <c r="S18" s="29"/>
+      <c r="T18" s="29"/>
     </row>
     <row r="19" spans="16:20" x14ac:dyDescent="0.2">
-      <c r="P19" s="30"/>
-      <c r="Q19" s="30"/>
-      <c r="R19" s="30"/>
-      <c r="S19" s="30"/>
-      <c r="T19" s="30"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="29"/>
+      <c r="R19" s="29"/>
+      <c r="S19" s="29"/>
+      <c r="T19" s="29"/>
     </row>
     <row r="20" spans="16:20" x14ac:dyDescent="0.2">
-      <c r="P20" s="30"/>
-      <c r="Q20" s="30"/>
-      <c r="R20" s="30"/>
-      <c r="S20" s="30"/>
-      <c r="T20" s="30"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="29"/>
+      <c r="R20" s="29"/>
+      <c r="S20" s="29"/>
+      <c r="T20" s="29"/>
     </row>
     <row r="21" spans="16:20" x14ac:dyDescent="0.2">
-      <c r="P21" s="30"/>
-      <c r="Q21" s="30"/>
-      <c r="R21" s="30"/>
-      <c r="S21" s="30"/>
-      <c r="T21" s="30"/>
+      <c r="P21" s="29"/>
+      <c r="Q21" s="29"/>
+      <c r="R21" s="29"/>
+      <c r="S21" s="29"/>
+      <c r="T21" s="29"/>
     </row>
     <row r="22" spans="16:20" x14ac:dyDescent="0.2">
-      <c r="P22" s="30"/>
-      <c r="Q22" s="30"/>
-      <c r="R22" s="30"/>
-      <c r="S22" s="30"/>
-      <c r="T22" s="30"/>
+      <c r="P22" s="29"/>
+      <c r="Q22" s="29"/>
+      <c r="R22" s="29"/>
+      <c r="S22" s="29"/>
+      <c r="T22" s="29"/>
     </row>
     <row r="23" spans="16:20" x14ac:dyDescent="0.2">
-      <c r="P23" s="30"/>
-      <c r="Q23" s="30"/>
-      <c r="R23" s="30"/>
-      <c r="S23" s="30"/>
-      <c r="T23" s="30"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="29"/>
+      <c r="R23" s="29"/>
+      <c r="S23" s="29"/>
+      <c r="T23" s="29"/>
     </row>
     <row r="24" spans="16:20" x14ac:dyDescent="0.2">
-      <c r="P24" s="30"/>
-      <c r="Q24" s="30"/>
-      <c r="R24" s="30"/>
-      <c r="S24" s="30"/>
-      <c r="T24" s="30"/>
+      <c r="P24" s="29"/>
+      <c r="Q24" s="29"/>
+      <c r="R24" s="29"/>
+      <c r="S24" s="29"/>
+      <c r="T24" s="29"/>
     </row>
     <row r="25" spans="16:20" x14ac:dyDescent="0.2">
-      <c r="P25" s="30"/>
-      <c r="Q25" s="30"/>
-      <c r="R25" s="30"/>
-      <c r="S25" s="30"/>
-      <c r="T25" s="30"/>
+      <c r="P25" s="29"/>
+      <c r="Q25" s="29"/>
+      <c r="R25" s="29"/>
+      <c r="S25" s="29"/>
+      <c r="T25" s="29"/>
     </row>
     <row r="26" spans="16:20" x14ac:dyDescent="0.2">
-      <c r="P26" s="30"/>
-      <c r="Q26" s="30"/>
-      <c r="R26" s="30"/>
-      <c r="S26" s="30"/>
-      <c r="T26" s="30"/>
+      <c r="P26" s="29"/>
+      <c r="Q26" s="29"/>
+      <c r="R26" s="29"/>
+      <c r="S26" s="29"/>
+      <c r="T26" s="29"/>
     </row>
     <row r="27" spans="16:20" x14ac:dyDescent="0.2">
-      <c r="P27" s="30"/>
-      <c r="Q27" s="30"/>
-      <c r="R27" s="30"/>
-      <c r="S27" s="30"/>
-      <c r="T27" s="30"/>
+      <c r="P27" s="29"/>
+      <c r="Q27" s="29"/>
+      <c r="R27" s="29"/>
+      <c r="S27" s="29"/>
+      <c r="T27" s="29"/>
     </row>
     <row r="28" spans="16:20" x14ac:dyDescent="0.2">
-      <c r="P28" s="30"/>
-      <c r="Q28" s="30"/>
-      <c r="R28" s="30"/>
-      <c r="S28" s="30"/>
-      <c r="T28" s="30"/>
+      <c r="P28" s="29"/>
+      <c r="Q28" s="29"/>
+      <c r="R28" s="29"/>
+      <c r="S28" s="29"/>
+      <c r="T28" s="29"/>
     </row>
     <row r="29" spans="16:20" x14ac:dyDescent="0.2">
-      <c r="P29" s="30"/>
-      <c r="Q29" s="30"/>
-      <c r="R29" s="30"/>
-      <c r="S29" s="30"/>
-      <c r="T29" s="30"/>
+      <c r="P29" s="29"/>
+      <c r="Q29" s="29"/>
+      <c r="R29" s="29"/>
+      <c r="S29" s="29"/>
+      <c r="T29" s="29"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1">
-    <cfRule type="duplicateValues" dxfId="35" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6260,10 +6432,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B2">
-    <cfRule type="duplicateValues" dxfId="34" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="33" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6330,7 +6502,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="32" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6398,7 +6570,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="52" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6641,7 +6813,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="31" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6673,7 +6845,7 @@
       <c r="A2" s="15" t="s">
         <v>482</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>476</v>
       </c>
     </row>
@@ -8362,9 +8534,11 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94216276-993F-46D5-B5DC-2B44F8AC08FA}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:A33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8604,12 +8778,47 @@
         <v>488</v>
       </c>
     </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
+        <v>554</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>556</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="30" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:A29">
-    <cfRule type="duplicateValues" dxfId="29" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30:A33">
+    <cfRule type="duplicateValues" dxfId="31" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8677,10 +8886,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A2">
-    <cfRule type="duplicateValues" dxfId="51" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="50" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8688,9 +8897,11 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838D319D-4E21-4D24-B515-3B21CF708CB5}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:A33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8930,12 +9141,47 @@
         <v>490</v>
       </c>
     </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
+        <v>554</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>556</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="28" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:A29">
-    <cfRule type="duplicateValues" dxfId="27" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30:A33">
+    <cfRule type="duplicateValues" dxfId="28" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8943,10 +9189,10 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{503541A4-E68E-4BF4-89DE-3D69378B1D9F}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="A16" sqref="A16:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8981,7 +9227,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>466</v>
@@ -8989,15 +9235,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>466</v>
@@ -9005,23 +9251,23 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>312</v>
+        <v>548</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>465</v>
@@ -9029,47 +9275,47 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>465</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>379</v>
+      <c r="A13" s="1" t="s">
+        <v>313</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>465</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>379</v>
+      <c r="A14" s="1" t="s">
+        <v>314</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>380</v>
+      <c r="A15" s="1" t="s">
+        <v>315</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>465</v>
@@ -9077,7 +9323,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>384</v>
+        <v>553</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>466</v>
@@ -9085,21 +9331,38 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>385</v>
+        <v>554</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>465</v>
       </c>
     </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>556</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>465</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="26" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13:A17">
-    <cfRule type="duplicateValues" dxfId="25" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B2">
-    <cfRule type="duplicateValues" dxfId="24" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16:A19">
+    <cfRule type="duplicateValues" dxfId="25" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9107,10 +9370,10 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E0D754A-7366-44A6-B051-72C1244AB996}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="A15" sqref="A15:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9139,7 +9402,7 @@
       <c r="A3" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="1" t="s">
         <v>455</v>
       </c>
     </row>
@@ -9147,227 +9410,138 @@
       <c r="A4" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="B4" s="19" t="s">
-        <v>455</v>
+      <c r="B4" s="1" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="B5" s="19" t="s">
+        <v>307</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>455</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="B6" s="25"/>
+        <v>308</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="B7" s="19" t="s">
+        <v>308</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>455</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="B8" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>454</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>454</v>
+        <v>310</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="B10" s="25"/>
+        <v>311</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>455</v>
+        <v>312</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B14" s="1" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>374</v>
-      </c>
-      <c r="B13" s="25"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="B14" s="25"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="B15" s="25"/>
+        <v>553</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>455</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>376</v>
-      </c>
-      <c r="B16" s="25"/>
+        <v>554</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>377</v>
-      </c>
-      <c r="B17" s="25"/>
+        <v>555</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>455</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>379</v>
-      </c>
-      <c r="B18" s="25"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
-        <v>380</v>
-      </c>
-      <c r="B19" s="25"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
-        <v>381</v>
-      </c>
-      <c r="B20" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
-        <v>382</v>
-      </c>
-      <c r="B21" s="25"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
-        <v>383</v>
-      </c>
-      <c r="B22" s="25"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="B23" s="25"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
-        <v>385</v>
-      </c>
-      <c r="B24" s="25"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
-        <v>387</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
-        <v>387</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
-        <v>389</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
-        <v>389</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
-        <v>388</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
-        <v>388</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
-        <v>390</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
-        <v>390</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>455</v>
-      </c>
-    </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="A15:A18">
+    <cfRule type="duplicateValues" dxfId="24" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3593EFF-45F7-4A29-8DE9-45EA98503C83}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:A16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9473,158 +9647,42 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>374</v>
+        <v>553</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>375</v>
+        <v>554</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>378</v>
+        <v>555</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>376</v>
+        <v>556</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>377</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>379</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
-        <v>380</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
-        <v>381</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
-        <v>382</v>
-      </c>
-      <c r="B21" s="1" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
-        <v>383</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
-        <v>385</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
-        <v>387</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
-        <v>389</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
-        <v>388</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
-        <v>390</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="6"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="6"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="6"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="6"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="23" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A13:A29">
-    <cfRule type="duplicateValues" dxfId="22" priority="2"/>
+  <conditionalFormatting sqref="A13:A16">
+    <cfRule type="duplicateValues" dxfId="22" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9632,10 +9690,10 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C62A5FFB-C134-40B1-8680-30D60A8885DF}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9643,7 +9701,7 @@
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>418</v>
       </c>
@@ -9651,7 +9709,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>417</v>
       </c>
@@ -9659,7 +9717,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>306</v>
       </c>
@@ -9667,7 +9725,7 @@
         <v>640640</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>307</v>
       </c>
@@ -9675,7 +9733,7 @@
         <v>500500</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>308</v>
       </c>
@@ -9683,7 +9741,7 @@
         <v>5001000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>309</v>
       </c>
@@ -9691,7 +9749,7 @@
         <v>512512</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>310</v>
       </c>
@@ -9699,15 +9757,15 @@
         <v>576576</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>311</v>
       </c>
       <c r="B8" s="6">
-        <v>640576</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>640640</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>312</v>
       </c>
@@ -9715,7 +9773,7 @@
         <v>640480</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>313</v>
       </c>
@@ -9723,7 +9781,7 @@
         <v>320160</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>314</v>
       </c>
@@ -9731,7 +9789,7 @@
         <v>960960</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>315</v>
       </c>
@@ -9739,186 +9797,74 @@
         <v>960960</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>374</v>
+        <v>553</v>
       </c>
       <c r="B13" s="6">
-        <v>480480</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>375</v>
+        <v>554</v>
       </c>
       <c r="B14" s="6">
-        <v>500500</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>378</v>
+        <v>555</v>
       </c>
       <c r="B15" s="6">
-        <v>5001000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>376</v>
+        <v>556</v>
       </c>
       <c r="B16" s="6">
-        <v>512512</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>377</v>
-      </c>
-      <c r="B17" s="6">
-        <v>576576</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>379</v>
-      </c>
-      <c r="B18" s="6">
-        <v>640640</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
-        <v>380</v>
-      </c>
-      <c r="B19" s="6">
-        <v>640640</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
-        <v>381</v>
-      </c>
-      <c r="B20" s="6">
-        <v>640480</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
-        <v>382</v>
-      </c>
-      <c r="B21" s="6">
-        <v>960960</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
-        <v>383</v>
-      </c>
-      <c r="B22" s="6">
-        <v>9601120</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="B23" s="6">
-        <v>960960</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
-        <v>385</v>
-      </c>
-      <c r="B24" s="6">
-        <v>960960</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="B25" s="6">
-        <v>960960</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
-        <v>387</v>
-      </c>
-      <c r="B26" s="6">
-        <v>500500</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
-        <v>389</v>
-      </c>
-      <c r="B27" s="6">
-        <v>500500</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
-        <v>388</v>
-      </c>
-      <c r="B28" s="6">
-        <v>5001000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
-        <v>390</v>
-      </c>
-      <c r="B29" s="6">
-        <v>5001000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F30" s="6"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F31" s="9"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F32" s="6"/>
-    </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F33" s="6"/>
-    </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F34" s="6"/>
-    </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F35" s="6"/>
-    </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F36" s="6"/>
-    </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F37" s="6"/>
-    </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F38" s="6"/>
-    </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F39" s="6"/>
-    </row>
-    <row r="40" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F40" s="6"/>
-    </row>
-    <row r="41" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F41" s="6"/>
-    </row>
-    <row r="42" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F42" s="6"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F25" s="6"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="21" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A13:A29">
+  <conditionalFormatting sqref="A13:A16">
     <cfRule type="duplicateValues" dxfId="20" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9928,23 +9874,25 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{330D0EDA-4CC0-4D25-885C-C1C08E778A60}">
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41:L45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="9.140625" style="1"/>
+    <col min="3" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="45" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="9" style="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="1" hidden="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>418</v>
       </c>
@@ -9952,7 +9900,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>417</v>
       </c>
@@ -9960,560 +9908,387 @@
         <v>246</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="B3" s="19"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="31"/>
+      <c r="O3" s="31"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="31"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="31"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="31"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="31"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="31"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="31"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="B4" s="19"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E10" s="32"/>
+      <c r="K10" s="32"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E11" s="32"/>
+      <c r="K11" s="32"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E12" s="32"/>
+      <c r="K12" s="32"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="E13" s="32"/>
+      <c r="K13" s="32"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="B5" s="19"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="B6" s="19"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="B14" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="B7" s="19"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="B18" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="B8" s="19"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="B20" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B9" s="19"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="B10" s="19"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="B25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="35"/>
+      <c r="L25" s="33"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="34"/>
+      <c r="L26" s="34"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="34"/>
+      <c r="L27" s="34"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="34"/>
+      <c r="L28" s="34"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="34"/>
+      <c r="L29" s="34"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E30" s="34"/>
+      <c r="L30" s="34"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E31" s="34"/>
+      <c r="L31" s="34"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E32" s="34"/>
+      <c r="L32" s="34"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E33" s="34"/>
+      <c r="L33" s="34"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>314</v>
-      </c>
-      <c r="B11" s="19"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="B12" s="19"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>374</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>374</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
-        <v>376</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
-        <v>376</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="s">
-        <v>376</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="6" t="s">
-        <v>376</v>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>314</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
-        <v>377</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>314</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
-        <v>377</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>314</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="6" t="s">
-        <v>379</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>314</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="6" t="s">
-        <v>379</v>
-      </c>
-      <c r="B39" s="1" t="s">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="6" t="s">
-        <v>379</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="6" t="s">
-        <v>379</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="6" t="s">
-        <v>379</v>
+      <c r="E41" s="36"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>315</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="6" t="s">
-        <v>379</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>315</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="6" t="s">
-        <v>380</v>
-      </c>
-      <c r="B44" s="19"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="6" t="s">
-        <v>381</v>
-      </c>
-      <c r="B45" s="19"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="6" t="s">
-        <v>382</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="6" t="s">
-        <v>382</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="6" t="s">
-        <v>382</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="6" t="s">
-        <v>382</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="6" t="s">
-        <v>382</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="6" t="s">
-        <v>383</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="6" t="s">
-        <v>383</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="6" t="s">
-        <v>383</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="6" t="s">
-        <v>383</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="6" t="s">
-        <v>383</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" s="6" t="s">
-        <v>385</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" s="6" t="s">
-        <v>385</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" s="6" t="s">
-        <v>385</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" s="6" t="s">
-        <v>385</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" s="6" t="s">
-        <v>385</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="6" t="s">
-        <v>387</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" s="6" t="s">
-        <v>389</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="6" t="s">
-        <v>388</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" s="6" t="s">
-        <v>390</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>143</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>557</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -11032,10 +10807,10 @@
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAADBBE6-1391-4512-B020-56872804993A}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B13"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11088,74 +10863,54 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
-        <v>512512</v>
+        <v>576576</v>
       </c>
       <c r="B6" s="6">
-        <v>256128</v>
+        <v>192192</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
-        <v>576576</v>
+        <v>640480</v>
       </c>
       <c r="B7" s="6">
-        <v>192192</v>
+        <v>320160</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
-        <v>640576</v>
+        <v>320160</v>
       </c>
       <c r="B8" s="6">
-        <v>320192</v>
+        <v>320160</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
-        <v>640480</v>
+        <v>960960</v>
       </c>
       <c r="B9" s="6">
         <v>320160</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
-        <v>320160</v>
-      </c>
-      <c r="B10" s="6">
-        <v>320160</v>
-      </c>
-    </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
-        <v>960960</v>
-      </c>
-      <c r="B11" s="6">
-        <v>320160</v>
-      </c>
+      <c r="A11"/>
+      <c r="B11"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
-        <v>480480</v>
-      </c>
-      <c r="B12" s="6">
-        <v>160160</v>
-      </c>
+      <c r="A12"/>
+      <c r="B12"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
-        <v>9601120</v>
-      </c>
-      <c r="B13" s="6">
-        <v>320160</v>
-      </c>
+      <c r="B13"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B14"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15"/>
       <c r="B15"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16"/>
       <c r="B16"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -11180,15 +10935,19 @@
       <c r="B23"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24"/>
       <c r="B24"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25"/>
       <c r="B25"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26"/>
       <c r="B26"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27"/>
       <c r="B27"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -11234,22 +10993,6 @@
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38"/>
       <c r="B38"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39"/>
-      <c r="B39"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40"/>
-      <c r="B40"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41"/>
-      <c r="B41"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42"/>
-      <c r="B42"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
@@ -11340,7 +11083,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A2">
     <cfRule type="duplicateValues" dxfId="14" priority="1"/>
   </conditionalFormatting>
@@ -11410,7 +11153,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="49" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11420,8 +11163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E20C1A-8A21-41E0-9FF7-195B3A3BE931}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AL56" sqref="AL56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13651,7 +13394,7 @@
       <c r="A3" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="B3" s="27">
+      <c r="B3" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13659,7 +13402,7 @@
       <c r="A4" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="B4" s="27">
+      <c r="B4" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13667,7 +13410,7 @@
       <c r="A5" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="B5" s="27">
+      <c r="B5" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13675,7 +13418,7 @@
       <c r="A6" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13683,7 +13426,7 @@
       <c r="A7" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="B7" s="27">
+      <c r="B7" s="26">
         <v>192192</v>
       </c>
     </row>
@@ -13691,7 +13434,7 @@
       <c r="A8" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="B8" s="27">
+      <c r="B8" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13699,7 +13442,7 @@
       <c r="A9" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="B9" s="27">
+      <c r="B9" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13707,7 +13450,7 @@
       <c r="A10" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="B10" s="27">
+      <c r="B10" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13715,7 +13458,7 @@
       <c r="A11" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="B11" s="27">
+      <c r="B11" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13723,7 +13466,7 @@
       <c r="A12" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="B12" s="27">
+      <c r="B12" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13731,7 +13474,7 @@
       <c r="A13" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="B13" s="27">
+      <c r="B13" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13739,7 +13482,7 @@
       <c r="A14" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="B14" s="27">
+      <c r="B14" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13747,7 +13490,7 @@
       <c r="A15" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="B15" s="27">
+      <c r="B15" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13755,7 +13498,7 @@
       <c r="A16" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="B16" s="27">
+      <c r="B16" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13763,7 +13506,7 @@
       <c r="A17" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="B17" s="27">
+      <c r="B17" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13771,7 +13514,7 @@
       <c r="A18" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="B18" s="27">
+      <c r="B18" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13779,7 +13522,7 @@
       <c r="A19" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="B19" s="27">
+      <c r="B19" s="26">
         <v>192192</v>
       </c>
     </row>
@@ -13787,7 +13530,7 @@
       <c r="A20" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="B20" s="27">
+      <c r="B20" s="26">
         <v>192192</v>
       </c>
     </row>
@@ -13795,7 +13538,7 @@
       <c r="A21" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="B21" s="27">
+      <c r="B21" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13803,7 +13546,7 @@
       <c r="A22" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="B22" s="27">
+      <c r="B22" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13811,7 +13554,7 @@
       <c r="A23" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="B23" s="27">
+      <c r="B23" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13819,7 +13562,7 @@
       <c r="A24" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="B24" s="27">
+      <c r="B24" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13827,7 +13570,7 @@
       <c r="A25" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="B25" s="27">
+      <c r="B25" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13835,7 +13578,7 @@
       <c r="A26" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="B26" s="27">
+      <c r="B26" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13843,7 +13586,7 @@
       <c r="A27" s="6" t="s">
         <v>340</v>
       </c>
-      <c r="B27" s="27">
+      <c r="B27" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13851,7 +13594,7 @@
       <c r="A28" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="B28" s="27">
+      <c r="B28" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13859,7 +13602,7 @@
       <c r="A29" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="B29" s="27">
+      <c r="B29" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13867,7 +13610,7 @@
       <c r="A30" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="B30" s="27">
+      <c r="B30" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13875,7 +13618,7 @@
       <c r="A31" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="B31" s="27">
+      <c r="B31" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13883,7 +13626,7 @@
       <c r="A32" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="B32" s="27">
+      <c r="B32" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13891,7 +13634,7 @@
       <c r="A33" s="6" t="s">
         <v>437</v>
       </c>
-      <c r="B33" s="27">
+      <c r="B33" s="26">
         <v>250250</v>
       </c>
     </row>
@@ -13899,7 +13642,7 @@
       <c r="A34" s="6" t="s">
         <v>435</v>
       </c>
-      <c r="B34" s="27">
+      <c r="B34" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13907,7 +13650,7 @@
       <c r="A35" s="6" t="s">
         <v>438</v>
       </c>
-      <c r="B35" s="27">
+      <c r="B35" s="26">
         <v>250250</v>
       </c>
     </row>
@@ -13915,7 +13658,7 @@
       <c r="A36" s="6" t="s">
         <v>439</v>
       </c>
-      <c r="B36" s="27">
+      <c r="B36" s="26">
         <v>250250</v>
       </c>
     </row>
@@ -13923,7 +13666,7 @@
       <c r="A37" s="6" t="s">
         <v>440</v>
       </c>
-      <c r="B37" s="27">
+      <c r="B37" s="26">
         <v>250250</v>
       </c>
     </row>
@@ -13931,7 +13674,7 @@
       <c r="A38" s="6" t="s">
         <v>441</v>
       </c>
-      <c r="B38" s="27">
+      <c r="B38" s="26">
         <v>250250</v>
       </c>
     </row>
@@ -13939,7 +13682,7 @@
       <c r="A39" s="6" t="s">
         <v>442</v>
       </c>
-      <c r="B39" s="27">
+      <c r="B39" s="26">
         <v>250250</v>
       </c>
     </row>
@@ -13947,7 +13690,7 @@
       <c r="A40" s="6" t="s">
         <v>443</v>
       </c>
-      <c r="B40" s="27">
+      <c r="B40" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13955,7 +13698,7 @@
       <c r="A41" s="6" t="s">
         <v>444</v>
       </c>
-      <c r="B41" s="27">
+      <c r="B41" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13963,7 +13706,7 @@
       <c r="A42" s="6" t="s">
         <v>445</v>
       </c>
-      <c r="B42" s="27">
+      <c r="B42" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -13971,7 +13714,7 @@
       <c r="A43" s="6" t="s">
         <v>446</v>
       </c>
-      <c r="B43" s="27">
+      <c r="B43" s="26">
         <v>240120</v>
       </c>
     </row>
@@ -13979,7 +13722,7 @@
       <c r="A44" s="6" t="s">
         <v>447</v>
       </c>
-      <c r="B44" s="27">
+      <c r="B44" s="26">
         <v>240120</v>
       </c>
     </row>
@@ -13987,7 +13730,7 @@
       <c r="A45" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="B45" s="27">
+      <c r="B45" s="26">
         <v>320160</v>
       </c>
     </row>
@@ -14848,7 +14591,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A2">
     <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
@@ -14882,10 +14625,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>476</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>478</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -14905,7 +14648,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="48" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14937,7 +14680,7 @@
       <c r="T2" s="15" t="s">
         <v>416</v>
       </c>
-      <c r="U2" s="26" t="s">
+      <c r="U2" s="25" t="s">
         <v>476</v>
       </c>
     </row>
@@ -15563,10 +15306,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>529</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>528</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -15619,7 +15362,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="47" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15697,7 +15440,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="46" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16082,7 +15825,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="45" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16114,10 +15857,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>515</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>252</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -16125,10 +15868,10 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="28">
+      <c r="A3" s="27">
         <v>1920</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="27">
         <v>1920</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -16136,10 +15879,10 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="28">
+      <c r="A4" s="27">
         <v>2880</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="27">
         <v>2880</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -16147,10 +15890,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="28">
+      <c r="A5" s="27">
         <v>3840</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="27">
         <v>3840</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -16158,10 +15901,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="28">
+      <c r="A6" s="27">
         <v>6000</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="27">
         <v>6000</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -16169,10 +15912,10 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="28">
+      <c r="A7" s="27">
         <v>7680</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="27">
         <v>7680</v>
       </c>
       <c r="C7" s="6" t="s">

</xml_diff>

<commit_message>
update with Brightness, Refresh, Module and Cabinet. Seems like inputs done!
</commit_message>
<xml_diff>
--- a/backend/data/database.xlsx
+++ b/backend/data/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\ledts\calculator\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B880FABC-D22A-4FF1-AFEF-930C5F4939F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7FA30BF-BF45-4057-8496-376939DF2443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="1000" firstSheet="13" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="1000" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="screen_type" sheetId="22" r:id="rId1"/>
@@ -4176,7 +4176,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:XFD45"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12612,7 +12612,7 @@
   <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+      <selection sqref="A1:B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15847,7 +15847,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C7"/>
+      <selection sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Check backend and frontend for Inputs. Regresh the seed file.
</commit_message>
<xml_diff>
--- a/backend/data/database.xlsx
+++ b/backend/data/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\ledts\calculator\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7FA30BF-BF45-4057-8496-376939DF2443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C6E089-6103-4C2C-B1EF-541FAF2A2B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="1000" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="1000" firstSheet="41" activeTab="50" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="screen_type" sheetId="22" r:id="rId1"/>
@@ -4175,7 +4175,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1557351-AC75-4275-84AC-10988B807ED9}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
@@ -14779,7 +14779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E32B68E-D42B-4786-BFE5-4B2187F4D12D}">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P49" sqref="P49"/>
     </sheetView>
   </sheetViews>
@@ -15462,7 +15462,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C33"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15501,7 +15501,7 @@
         <v>0.8</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -15512,7 +15512,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -15534,7 +15534,7 @@
         <v>1.37</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -15578,7 +15578,7 @@
         <v>1.87</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -15622,7 +15622,7 @@
         <v>2.97</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -15666,7 +15666,7 @@
         <v>3.91</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -15688,7 +15688,7 @@
         <v>4.46</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -15699,7 +15699,7 @@
         <v>4.8099999999999996</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -15721,7 +15721,7 @@
         <v>5.21</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -15743,7 +15743,7 @@
         <v>6.25</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -15765,7 +15765,7 @@
         <v>6.67</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -15798,7 +15798,7 @@
         <v>8.91</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -15809,7 +15809,7 @@
         <v>10</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -15820,7 +15820,7 @@
         <v>13.33</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -15831,7 +15831,7 @@
         <v>16</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Backend update foк module Details and Cabinet Details
</commit_message>
<xml_diff>
--- a/backend/data/database.xlsx
+++ b/backend/data/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\ledts\calculator\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C6E089-6103-4C2C-B1EF-541FAF2A2B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B598949-C378-4ED6-9575-DE225D6922F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="1000" firstSheet="41" activeTab="50" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25590" yWindow="0" windowWidth="26010" windowHeight="20880" tabRatio="1000" firstSheet="15" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="screen_type" sheetId="22" r:id="rId1"/>
@@ -4827,8 +4827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A087147-0889-47E2-B7E5-6733E2DA4BB8}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:A33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5328,7 +5328,7 @@
   <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5568,10 +5568,10 @@
         <v>576576</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="R7" s="6">
-        <v>640</v>
+        <v>576</v>
       </c>
       <c r="S7" s="6">
         <v>576</v>
@@ -10821,7 +10821,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14779,7 +14779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E32B68E-D42B-4786-BFE5-4B2187F4D12D}">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P49" sqref="P49"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update to beat the backend and open the Drewer
</commit_message>
<xml_diff>
--- a/backend/data/database.xlsx
+++ b/backend/data/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\ledts\calculator\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B598949-C378-4ED6-9575-DE225D6922F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C85EA1-DC12-4D03-990D-DF64C1E9B003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25590" yWindow="0" windowWidth="26010" windowHeight="20880" tabRatio="1000" firstSheet="15" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25590" yWindow="0" windowWidth="26010" windowHeight="20880" tabRatio="1000" firstSheet="31" activeTab="34" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="screen_type" sheetId="22" r:id="rId1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2602" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2602" uniqueCount="574">
   <si>
     <t>уличный</t>
   </si>
@@ -1685,15 +1685,6 @@
     <t>512x1000</t>
   </si>
   <si>
-    <t>576x512</t>
-  </si>
-  <si>
-    <t>320x480</t>
-  </si>
-  <si>
-    <t>960x160</t>
-  </si>
-  <si>
     <t>module_name</t>
   </si>
   <si>
@@ -1827,6 +1818,9 @@
   </si>
   <si>
     <t>QIANGLI, Q2,5 (320*160) 6000hz,indoor,гибкий</t>
+  </si>
+  <si>
+    <t>6400x480</t>
   </si>
 </sst>
 </file>
@@ -4193,7 +4187,7 @@
         <v>402</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>238</v>
@@ -4207,7 +4201,7 @@
         <v>403</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>147</v>
@@ -4221,7 +4215,7 @@
         <v>316</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>152</v>
@@ -4235,7 +4229,7 @@
         <v>317</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>153</v>
@@ -4249,7 +4243,7 @@
         <v>318</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>154</v>
@@ -4263,7 +4257,7 @@
         <v>319</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>155</v>
@@ -4277,7 +4271,7 @@
         <v>320</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>156</v>
@@ -4291,7 +4285,7 @@
         <v>321</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>157</v>
@@ -4305,7 +4299,7 @@
         <v>322</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>158</v>
@@ -4319,7 +4313,7 @@
         <v>323</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>159</v>
@@ -4333,7 +4327,7 @@
         <v>324</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>160</v>
@@ -4347,7 +4341,7 @@
         <v>325</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>161</v>
@@ -4361,7 +4355,7 @@
         <v>326</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>162</v>
@@ -4375,7 +4369,7 @@
         <v>327</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>163</v>
@@ -4389,7 +4383,7 @@
         <v>328</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>164</v>
@@ -4403,7 +4397,7 @@
         <v>329</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>165</v>
@@ -4417,7 +4411,7 @@
         <v>330</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>166</v>
@@ -4431,7 +4425,7 @@
         <v>331</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>167</v>
@@ -4445,7 +4439,7 @@
         <v>332</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>168</v>
@@ -4459,7 +4453,7 @@
         <v>333</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>169</v>
@@ -4473,7 +4467,7 @@
         <v>334</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>170</v>
@@ -4487,7 +4481,7 @@
         <v>335</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>171</v>
@@ -4501,7 +4495,7 @@
         <v>336</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>172</v>
@@ -4515,7 +4509,7 @@
         <v>337</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>173</v>
@@ -4529,7 +4523,7 @@
         <v>338</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>174</v>
@@ -4543,7 +4537,7 @@
         <v>339</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>175</v>
@@ -4557,7 +4551,7 @@
         <v>340</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>176</v>
@@ -4571,7 +4565,7 @@
         <v>341</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>177</v>
@@ -4585,7 +4579,7 @@
         <v>342</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>178</v>
@@ -4599,7 +4593,7 @@
         <v>343</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>179</v>
@@ -4613,7 +4607,7 @@
         <v>344</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>180</v>
@@ -4627,7 +4621,7 @@
         <v>345</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>181</v>
@@ -4769,7 +4763,7 @@
         <v>256128</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C7" s="3">
         <v>256</v>
@@ -4786,7 +4780,7 @@
         <v>320192</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="C8" s="6">
         <v>320</v>
@@ -4803,7 +4797,7 @@
         <v>160160</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="C9" s="6">
         <v>160</v>
@@ -4827,8 +4821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A087147-0889-47E2-B7E5-6733E2DA4BB8}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5247,13 +5241,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>398</v>
@@ -5261,13 +5255,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>398</v>
@@ -5275,13 +5269,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>398</v>
@@ -5289,13 +5283,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>398</v>
@@ -5328,7 +5322,7 @@
   <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5535,10 +5529,10 @@
         <v>512512</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>528</v>
+        <v>353</v>
       </c>
       <c r="R6" s="6">
-        <v>576</v>
+        <v>512</v>
       </c>
       <c r="S6" s="6">
         <v>512</v>
@@ -5634,10 +5628,10 @@
         <v>640480</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>529</v>
+        <v>573</v>
       </c>
       <c r="R9" s="6">
-        <v>320</v>
+        <v>640</v>
       </c>
       <c r="S9" s="6">
         <v>480</v>
@@ -5667,10 +5661,10 @@
         <v>320160</v>
       </c>
       <c r="Q10" s="6" t="s">
-        <v>530</v>
+        <v>357</v>
       </c>
       <c r="R10" s="6">
-        <v>960</v>
+        <v>320</v>
       </c>
       <c r="S10" s="6">
         <v>160</v>
@@ -8791,7 +8785,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>475</v>
@@ -8799,7 +8793,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>475</v>
@@ -8807,7 +8801,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>475</v>
@@ -8815,7 +8809,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>475</v>
@@ -9154,7 +9148,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>477</v>
@@ -9162,7 +9156,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>477</v>
@@ -9170,7 +9164,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>477</v>
@@ -9178,7 +9172,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>477</v>
@@ -9278,7 +9272,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>452</v>
@@ -9334,7 +9328,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>453</v>
@@ -9342,7 +9336,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>453</v>
@@ -9350,7 +9344,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>452</v>
@@ -9358,7 +9352,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>452</v>
@@ -9507,7 +9501,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>442</v>
@@ -9515,7 +9509,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>441</v>
@@ -9523,7 +9517,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>442</v>
@@ -9531,7 +9525,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>441</v>
@@ -9658,7 +9652,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>449</v>
@@ -9666,7 +9660,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>449</v>
@@ -9674,7 +9668,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>449</v>
@@ -9682,7 +9676,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>449</v>
@@ -9810,7 +9804,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B13" s="6">
         <v>0</v>
@@ -9819,7 +9813,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B14" s="6">
         <v>0</v>
@@ -9828,7 +9822,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B15" s="6">
         <v>0</v>
@@ -9837,7 +9831,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="B16" s="6">
         <v>0</v>
@@ -9887,8 +9881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{330D0EDA-4CC0-4D25-885C-C1C08E778A60}">
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41:L45"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10295,7 +10289,7 @@
         <v>315</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
   </sheetData>
@@ -10821,7 +10815,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13758,7 +13752,7 @@
   <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="A19" sqref="A19:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Drawer table visual update
</commit_message>
<xml_diff>
--- a/backend/data/database.xlsx
+++ b/backend/data/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\ledts\calculator\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C85EA1-DC12-4D03-990D-DF64C1E9B003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2812D4-821B-4DAA-9ABE-0FCF54721926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25590" yWindow="0" windowWidth="26010" windowHeight="20880" tabRatio="1000" firstSheet="31" activeTab="34" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25590" yWindow="0" windowWidth="26010" windowHeight="20880" tabRatio="1000" firstSheet="39" activeTab="48" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="screen_type" sheetId="22" r:id="rId1"/>
@@ -9881,7 +9881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{330D0EDA-4CC0-4D25-885C-C1C08E778A60}">
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -14518,8 +14518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF89E3F5-DCE7-44A2-8672-367DB4BDA25F}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14542,7 +14542,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>230</v>

</xml_diff>

<commit_message>
feat(calculator): Implement full calculation logic and fix dev environment
Successfully implemented the complete calculation flow, including additional services. Resolved all critical bugs related to the development environment, data loading, and type safety.

Key achievements:
- Added full-stack logic for Video Processors (DB, GraphQL, Frontend).
- Implemented calculation for additional services: montage, construction, delivery.
- Fixed all data loading issues (400 Bad Request) in the local dev environment by correcting Vite proxy and React Query hook configurations.
- Resolved all TypeScript compilation errors by enabling strict mode and correctly typing the entire backend and frontend data flow.
- Stabilized the local development server by fixing tsx hot-reloading loops.
- The calculator now correctly fetches, calculates, and displays all technical and cost parameters.
</commit_message>
<xml_diff>
--- a/backend/data/database.xlsx
+++ b/backend/data/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\ledts\calculator\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404D5D54-8CF6-4649-A6CE-D517C37E8F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2A1DDF-8C3A-44B3-A7C8-40F92424C477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="1000" firstSheet="30" activeTab="50" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="1000" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="screen_type" sheetId="22" r:id="rId1"/>
@@ -27,46 +27,47 @@
     <sheet name="supplier" sheetId="44" r:id="rId12"/>
     <sheet name="ip_protection" sheetId="4" r:id="rId13"/>
     <sheet name="module" sheetId="7" r:id="rId14"/>
-    <sheet name="module_size" sheetId="68" r:id="rId15"/>
-    <sheet name="cabinet" sheetId="43" r:id="rId16"/>
-    <sheet name="cabinet_size" sheetId="66" r:id="rId17"/>
-    <sheet name="item" sheetId="6" r:id="rId18"/>
-    <sheet name="item_category" sheetId="41" r:id="rId19"/>
-    <sheet name="item_subcategory" sheetId="42" r:id="rId20"/>
-    <sheet name="screen_type&gt;option" sheetId="64" r:id="rId21"/>
-    <sheet name="screen_type&gt;control_type" sheetId="89" r:id="rId22"/>
-    <sheet name="screen_type&gt;sensor" sheetId="88" r:id="rId23"/>
-    <sheet name="item&gt;category" sheetId="82" r:id="rId24"/>
-    <sheet name="item&gt;subcategory" sheetId="83" r:id="rId25"/>
-    <sheet name="item_category&gt;item_subcategory" sheetId="53" r:id="rId26"/>
-    <sheet name="item&gt;price" sheetId="85" r:id="rId27"/>
-    <sheet name="item&gt;supplier" sheetId="84" r:id="rId28"/>
-    <sheet name="cabinet&gt;category" sheetId="63" r:id="rId29"/>
-    <sheet name="cabinet&gt;subcategory" sheetId="65" r:id="rId30"/>
-    <sheet name="cabinet&gt;location" sheetId="58" r:id="rId31"/>
-    <sheet name="cabinet&gt;placement" sheetId="55" r:id="rId32"/>
-    <sheet name="cabinet&gt;material" sheetId="57" r:id="rId33"/>
-    <sheet name="cabinet&gt;cabinet_size" sheetId="67" r:id="rId34"/>
-    <sheet name="cabinet&gt;pitch" sheetId="54" r:id="rId35"/>
-    <sheet name="cabinet&gt;manufacturer" sheetId="60" r:id="rId36"/>
-    <sheet name="cabinet&gt;supplier" sheetId="59" r:id="rId37"/>
-    <sheet name="cabinet_size&gt;module_size" sheetId="69" r:id="rId38"/>
-    <sheet name="cabinet&gt;items_count" sheetId="17" r:id="rId39"/>
-    <sheet name="cabinet&gt;price" sheetId="75" r:id="rId40"/>
-    <sheet name="module&gt;category" sheetId="70" r:id="rId41"/>
-    <sheet name="module&gt;subcategory" sheetId="71" r:id="rId42"/>
-    <sheet name="module&gt;location" sheetId="72" r:id="rId43"/>
-    <sheet name="module&gt;refresh_rate" sheetId="80" r:id="rId44"/>
-    <sheet name="module&gt;brightness" sheetId="81" r:id="rId45"/>
-    <sheet name="module&gt;module_size" sheetId="76" r:id="rId46"/>
-    <sheet name="module&gt;pitch" sheetId="74" r:id="rId47"/>
-    <sheet name="module&gt;manufacturer" sheetId="73" r:id="rId48"/>
-    <sheet name="module&gt;items_count" sheetId="52" r:id="rId49"/>
-    <sheet name="module&gt;option" sheetId="61" r:id="rId50"/>
-    <sheet name="module&gt;price" sheetId="77" r:id="rId51"/>
+    <sheet name="video_processor" sheetId="90" r:id="rId15"/>
+    <sheet name="module_size" sheetId="68" r:id="rId16"/>
+    <sheet name="cabinet" sheetId="43" r:id="rId17"/>
+    <sheet name="cabinet_size" sheetId="66" r:id="rId18"/>
+    <sheet name="item" sheetId="6" r:id="rId19"/>
+    <sheet name="item_category" sheetId="41" r:id="rId20"/>
+    <sheet name="item_subcategory" sheetId="42" r:id="rId21"/>
+    <sheet name="screen_type&gt;option" sheetId="64" r:id="rId22"/>
+    <sheet name="screen_type&gt;control_type" sheetId="89" r:id="rId23"/>
+    <sheet name="screen_type&gt;sensor" sheetId="88" r:id="rId24"/>
+    <sheet name="item&gt;category" sheetId="82" r:id="rId25"/>
+    <sheet name="item&gt;subcategory" sheetId="83" r:id="rId26"/>
+    <sheet name="item_category&gt;item_subcategory" sheetId="53" r:id="rId27"/>
+    <sheet name="item&gt;price" sheetId="85" r:id="rId28"/>
+    <sheet name="item&gt;supplier" sheetId="84" r:id="rId29"/>
+    <sheet name="cabinet&gt;category" sheetId="63" r:id="rId30"/>
+    <sheet name="cabinet&gt;subcategory" sheetId="65" r:id="rId31"/>
+    <sheet name="cabinet&gt;location" sheetId="58" r:id="rId32"/>
+    <sheet name="cabinet&gt;placement" sheetId="55" r:id="rId33"/>
+    <sheet name="cabinet&gt;material" sheetId="57" r:id="rId34"/>
+    <sheet name="cabinet&gt;cabinet_size" sheetId="67" r:id="rId35"/>
+    <sheet name="cabinet&gt;pitch" sheetId="54" r:id="rId36"/>
+    <sheet name="cabinet&gt;manufacturer" sheetId="60" r:id="rId37"/>
+    <sheet name="cabinet&gt;supplier" sheetId="59" r:id="rId38"/>
+    <sheet name="cabinet_size&gt;module_size" sheetId="69" r:id="rId39"/>
+    <sheet name="cabinet&gt;items_count" sheetId="17" r:id="rId40"/>
+    <sheet name="cabinet&gt;price" sheetId="75" r:id="rId41"/>
+    <sheet name="module&gt;category" sheetId="70" r:id="rId42"/>
+    <sheet name="module&gt;subcategory" sheetId="71" r:id="rId43"/>
+    <sheet name="module&gt;location" sheetId="72" r:id="rId44"/>
+    <sheet name="module&gt;refresh_rate" sheetId="80" r:id="rId45"/>
+    <sheet name="module&gt;brightness" sheetId="81" r:id="rId46"/>
+    <sheet name="module&gt;module_size" sheetId="76" r:id="rId47"/>
+    <sheet name="module&gt;pitch" sheetId="74" r:id="rId48"/>
+    <sheet name="module&gt;manufacturer" sheetId="73" r:id="rId49"/>
+    <sheet name="module&gt;items_count" sheetId="52" r:id="rId50"/>
+    <sheet name="module&gt;option" sheetId="61" r:id="rId51"/>
+    <sheet name="module&gt;price" sheetId="77" r:id="rId52"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">cabinet!$A$2:$C$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">cabinet!$A$2:$C$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">module!$A$2:$D$32</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -87,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2230" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2314" uniqueCount="610">
   <si>
     <t>уличный</t>
   </si>
@@ -1734,6 +1735,189 @@
   </si>
   <si>
     <t>QIANGLI, Q2,5 (320*160) 6000hz,indoor,гибкий</t>
+  </si>
+  <si>
+    <t>processor_code</t>
+  </si>
+  <si>
+    <t>Код процессора</t>
+  </si>
+  <si>
+    <t>processor_name</t>
+  </si>
+  <si>
+    <t>processor_sku</t>
+  </si>
+  <si>
+    <t>Видео процессор NovaPro UHD JR</t>
+  </si>
+  <si>
+    <t>Видео процессор NovaPro UHD</t>
+  </si>
+  <si>
+    <t>Видео процессор VS7</t>
+  </si>
+  <si>
+    <t>Видео процессор VX400S-N</t>
+  </si>
+  <si>
+    <t>Видео процессор VX400</t>
+  </si>
+  <si>
+    <t>Видео процессор VX4S-N</t>
+  </si>
+  <si>
+    <t>Видео процессор VX600</t>
+  </si>
+  <si>
+    <t>Видео процессор VX16S</t>
+  </si>
+  <si>
+    <t>Медиа процессор TU15 Pro</t>
+  </si>
+  <si>
+    <t>Медиа процессор TU20 Pro</t>
+  </si>
+  <si>
+    <t>Медиа процессор TU40 Pro</t>
+  </si>
+  <si>
+    <t>Видео процессор VC4</t>
+  </si>
+  <si>
+    <t>Видео процессор VC6</t>
+  </si>
+  <si>
+    <t>Видео процессор VC10</t>
+  </si>
+  <si>
+    <t>Видео процессор VC16</t>
+  </si>
+  <si>
+    <t>Видео процессор VC24</t>
+  </si>
+  <si>
+    <t>Видео процессор VX1000</t>
+  </si>
+  <si>
+    <t>Видео процессор CX40 Pro</t>
+  </si>
+  <si>
+    <t>Видео процессор CX80 Pro</t>
+  </si>
+  <si>
+    <t>VP-NPUHD</t>
+  </si>
+  <si>
+    <t>VP-NPUHDJr</t>
+  </si>
+  <si>
+    <t>NPUHDJr</t>
+  </si>
+  <si>
+    <t>NPUHD</t>
+  </si>
+  <si>
+    <t>VP-VS7</t>
+  </si>
+  <si>
+    <t>VS7</t>
+  </si>
+  <si>
+    <t>VP-400SN</t>
+  </si>
+  <si>
+    <t>400SN</t>
+  </si>
+  <si>
+    <t>VP-VX400</t>
+  </si>
+  <si>
+    <t>VX400</t>
+  </si>
+  <si>
+    <t>VP-VX4S</t>
+  </si>
+  <si>
+    <t>VX4S</t>
+  </si>
+  <si>
+    <t>VP-VX6S</t>
+  </si>
+  <si>
+    <t>VX6S</t>
+  </si>
+  <si>
+    <t>VX16S</t>
+  </si>
+  <si>
+    <t>TU15</t>
+  </si>
+  <si>
+    <t>TU20</t>
+  </si>
+  <si>
+    <t>TU40</t>
+  </si>
+  <si>
+    <t>VC4</t>
+  </si>
+  <si>
+    <t>VC6</t>
+  </si>
+  <si>
+    <t>VC10</t>
+  </si>
+  <si>
+    <t>VC16</t>
+  </si>
+  <si>
+    <t>VC24</t>
+  </si>
+  <si>
+    <t>VX1000</t>
+  </si>
+  <si>
+    <t>CX40PRO</t>
+  </si>
+  <si>
+    <t>CX80PRO</t>
+  </si>
+  <si>
+    <t>VP-VX16S</t>
+  </si>
+  <si>
+    <t>MP-TU15</t>
+  </si>
+  <si>
+    <t>MP-TU20</t>
+  </si>
+  <si>
+    <t>MP-TU40</t>
+  </si>
+  <si>
+    <t>VP-VC4</t>
+  </si>
+  <si>
+    <t>VP-VC6</t>
+  </si>
+  <si>
+    <t>VP-VC10</t>
+  </si>
+  <si>
+    <t>VP-VC16</t>
+  </si>
+  <si>
+    <t>VP-VC24</t>
+  </si>
+  <si>
+    <t>VP-VX1000</t>
+  </si>
+  <si>
+    <t>VP-CX40PRO</t>
+  </si>
+  <si>
+    <t>VP-CX80PRO</t>
   </si>
 </sst>
 </file>
@@ -1867,7 +2051,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1957,6 +2141,17 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1966,7 +2161,17 @@
     <cellStyle name="Normal 5" xfId="4" xr:uid="{ED67CD53-254C-476B-A43A-A6D366E9B16E}"/>
     <cellStyle name="Normal 6" xfId="5" xr:uid="{31321808-6278-4398-B32B-0EC153BDC8A4}"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="53">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2899,7 +3104,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="43" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2976,7 +3181,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="42" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4008,7 +4213,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D2">
-    <cfRule type="duplicateValues" dxfId="41" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4024,7 +4229,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4488,7 +4693,7 @@
   <autoFilter ref="A2:D32" xr:uid="{D1557351-AC75-4275-84AC-10988B807ED9}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A2:B2">
-    <cfRule type="duplicateValues" dxfId="40" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4496,6 +4701,325 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE8B44D-D866-47D4-A9AE-7ACEC07979C3}">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="72.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" style="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="38" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" style="38" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="72.140625" style="38"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="38" t="s">
+        <v>549</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>551</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>552</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="40" t="s">
+        <v>550</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>518</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="38" t="s">
+        <v>574</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>553</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>573</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="38" t="s">
+        <v>575</v>
+      </c>
+      <c r="B4" s="41" t="s">
+        <v>554</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>572</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="38" t="s">
+        <v>577</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>555</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>576</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="38" t="s">
+        <v>579</v>
+      </c>
+      <c r="B6" s="41" t="s">
+        <v>556</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>578</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="38" t="s">
+        <v>581</v>
+      </c>
+      <c r="B7" s="41" t="s">
+        <v>557</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>580</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="38" t="s">
+        <v>583</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>558</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>582</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="38" t="s">
+        <v>585</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>559</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>584</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="38" t="s">
+        <v>586</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>560</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>598</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="38" t="s">
+        <v>587</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>561</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>599</v>
+      </c>
+      <c r="D11" s="38" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="38" t="s">
+        <v>588</v>
+      </c>
+      <c r="B12" s="41" t="s">
+        <v>562</v>
+      </c>
+      <c r="C12" s="41" t="s">
+        <v>600</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="38" t="s">
+        <v>589</v>
+      </c>
+      <c r="B13" s="41" t="s">
+        <v>563</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>601</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="38" t="s">
+        <v>590</v>
+      </c>
+      <c r="B14" s="41" t="s">
+        <v>564</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>602</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="38" t="s">
+        <v>591</v>
+      </c>
+      <c r="B15" s="41" t="s">
+        <v>565</v>
+      </c>
+      <c r="C15" s="41" t="s">
+        <v>603</v>
+      </c>
+      <c r="D15" s="38" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="38" t="s">
+        <v>592</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>566</v>
+      </c>
+      <c r="C16" s="41" t="s">
+        <v>604</v>
+      </c>
+      <c r="D16" s="38" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="38" t="s">
+        <v>593</v>
+      </c>
+      <c r="B17" s="41" t="s">
+        <v>567</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>605</v>
+      </c>
+      <c r="D17" s="38" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="38" t="s">
+        <v>594</v>
+      </c>
+      <c r="B18" s="41" t="s">
+        <v>568</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>606</v>
+      </c>
+      <c r="D18" s="38" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="38" t="s">
+        <v>595</v>
+      </c>
+      <c r="B19" s="41" t="s">
+        <v>569</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>607</v>
+      </c>
+      <c r="D19" s="38" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="38" t="s">
+        <v>596</v>
+      </c>
+      <c r="B20" s="41" t="s">
+        <v>570</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>608</v>
+      </c>
+      <c r="D20" s="38" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="38" t="s">
+        <v>597</v>
+      </c>
+      <c r="B21" s="41" t="s">
+        <v>571</v>
+      </c>
+      <c r="C21" s="41" t="s">
+        <v>609</v>
+      </c>
+      <c r="D21" s="38" t="s">
+        <v>381</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:B2">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2307915A-A735-4F12-9C66-1563AEDE7F84}">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -4665,13 +5189,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E2">
-    <cfRule type="duplicateValues" dxfId="39" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A087147-0889-47E2-B7E5-6733E2DA4BB8}">
   <dimension ref="A1:D16"/>
   <sheetViews>
@@ -4915,22 +5439,22 @@
   <autoFilter ref="A2:C12" xr:uid="{3A087147-0889-47E2-B7E5-6733E2DA4BB8}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="38" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:A16">
-    <cfRule type="duplicateValues" dxfId="37" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="36" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C2">
-    <cfRule type="duplicateValues" dxfId="35" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314C64C8-D764-439F-956B-E5FFD48CB80C}">
   <dimension ref="A1:T29"/>
   <sheetViews>
@@ -5493,13 +6017,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1">
-    <cfRule type="duplicateValues" dxfId="34" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C85276AB-6D20-4E24-BA3A-1994BA2758AE}">
   <dimension ref="A1:D38"/>
   <sheetViews>
@@ -6050,77 +6574,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B2">
-    <cfRule type="duplicateValues" dxfId="33" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="32" priority="2"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3A7BEE4-357A-4B65-BDAB-F5658C8BDDF7}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
-        <v>449</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>381</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="31" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6188,13 +6645,80 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="51" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3A7BEE4-357A-4B65-BDAB-F5658C8BDDF7}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>449</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>381</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C1:C2">
+    <cfRule type="duplicateValues" dxfId="32" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758A5D86-441E-4547-BFC0-37BF0DA3CA4E}">
   <dimension ref="A1:C20"/>
   <sheetViews>
@@ -6431,13 +6955,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="30" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDFA7EB3-932A-4811-830A-42A8E45E58AF}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -6480,7 +7004,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FA8A2D8-3256-440B-9E14-E258265742B7}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -6540,7 +7064,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314E267F-11E0-4E95-AEBA-94E96160A3C7}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -6608,7 +7132,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D160B1-107D-4062-8C86-03A4B392FA38}">
   <dimension ref="A1:B38"/>
   <sheetViews>
@@ -6931,7 +7455,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C04F08E6-C957-4635-AE71-6C74CA9C905B}">
   <dimension ref="A1:B38"/>
   <sheetViews>
@@ -7254,7 +7778,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D53FD8-1A25-412E-A323-F2F488E6171C}">
   <dimension ref="A1:C21"/>
   <sheetViews>
@@ -7463,7 +7987,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D49BE8BB-ED20-4228-91B2-2B60FBF78A05}">
   <dimension ref="A1:C38"/>
   <sheetViews>
@@ -7827,7 +8351,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB2A56E-17F5-4F4B-B55A-AC097B038314}">
   <dimension ref="A1:B38"/>
   <sheetViews>
@@ -8146,159 +8670,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94216276-993F-46D5-B5DC-2B44F8AC08FA}">
-  <dimension ref="A1:B16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>513</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>514</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>515</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>516</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="29" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13:A16">
-    <cfRule type="duplicateValues" dxfId="28" priority="1"/>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8365,16 +8736,169 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A2">
-    <cfRule type="duplicateValues" dxfId="50" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="49" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94216276-993F-46D5-B5DC-2B44F8AC08FA}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>513</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>514</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>515</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>516</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="duplicateValues" dxfId="30" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:A16">
+    <cfRule type="duplicateValues" dxfId="29" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838D319D-4E21-4D24-B515-3B21CF708CB5}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -8518,16 +9042,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="27" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:A16">
-    <cfRule type="duplicateValues" dxfId="26" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{503541A4-E68E-4BF4-89DE-3D69378B1D9F}">
   <dimension ref="A1:B19"/>
   <sheetViews>
@@ -8696,19 +9220,19 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="25" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:A19">
-    <cfRule type="duplicateValues" dxfId="24" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B2">
-    <cfRule type="duplicateValues" dxfId="23" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E0D754A-7366-44A6-B051-72C1244AB996}">
   <dimension ref="A1:B18"/>
   <sheetViews>
@@ -8869,13 +9393,13 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A15:A18">
-    <cfRule type="duplicateValues" dxfId="22" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3593EFF-45F7-4A29-8DE9-45EA98503C83}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -9019,16 +9543,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="21" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:A16">
-    <cfRule type="duplicateValues" dxfId="20" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C62A5FFB-C134-40B1-8680-30D60A8885DF}">
   <dimension ref="A1:F25"/>
   <sheetViews>
@@ -9202,17 +9726,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="19" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:A16">
-    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{330D0EDA-4CC0-4D25-885C-C1C08E778A60}">
   <dimension ref="A1:O45"/>
   <sheetViews>
@@ -9633,7 +10157,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0798065-59C6-4720-93E4-3CE4B33BD8CB}">
   <dimension ref="A1:B12"/>
   <sheetViews>
@@ -9745,13 +10269,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="17" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E91E25B2-4E92-4D46-9C6E-1BA2E58E750C}">
   <dimension ref="A1:B12"/>
   <sheetViews>
@@ -9863,13 +10387,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="16" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAADBBE6-1391-4512-B020-56872804993A}">
   <dimension ref="A1:E38"/>
   <sheetViews>
@@ -10060,96 +10584,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E240DF3-D7B4-41E6-94E7-4D5C366CEC52}">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
-        <v>386</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>230</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C3" s="16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="C5" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="16">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="14" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10217,13 +10652,102 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="48" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E240DF3-D7B4-41E6-94E7-4D5C366CEC52}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C3" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C5" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="16">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E20C1A-8A21-41E0-9FF7-195B3A3BE931}">
   <dimension ref="A1:C29"/>
   <sheetViews>
@@ -10505,17 +11029,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="13" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:A29">
-    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F173EB0-1826-43CD-BBC2-34F89B38C63B}">
   <dimension ref="A1:B33"/>
   <sheetViews>
@@ -10795,13 +11319,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6AED28-F84F-42E9-A39A-F30D0BC83333}">
   <dimension ref="A1:B33"/>
   <sheetViews>
@@ -11081,13 +11605,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41B1924F-8A91-4798-BDD8-22FF652F0B04}">
   <dimension ref="A1:B33"/>
   <sheetViews>
@@ -11367,13 +11891,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE4D75B-E407-4F92-A284-9A481483437D}">
   <dimension ref="A1:B33"/>
   <sheetViews>
@@ -11653,13 +12177,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A219D196-7B8E-4099-8625-180160D6F341}">
   <dimension ref="A1:B33"/>
   <sheetViews>
@@ -11939,13 +12463,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E9B45FD-FDD3-4BEC-879C-2FF139E7A735}">
   <dimension ref="A1:B33"/>
   <sheetViews>
@@ -12225,13 +12749,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E097EFF-1109-433D-8B8B-E3D27DAE80CB}">
   <dimension ref="A1:B33"/>
   <sheetViews>
@@ -12511,16 +13035,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B2">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AFA6094-3E85-4CD9-9B78-057F896D00E5}">
   <dimension ref="A1:B33"/>
   <sheetViews>
@@ -12800,97 +13324,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF89E3F5-DCE7-44A2-8672-367DB4BDA25F}">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
-        <v>386</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>230</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C3" s="16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="C5" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="16">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12945,13 +13379,103 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="47" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF89E3F5-DCE7-44A2-8672-367DB4BDA25F}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C3" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C5" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="16">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03257CC6-E027-4B24-8632-0554CE95F789}">
   <dimension ref="T1:U11"/>
   <sheetViews>
@@ -13055,18 +13579,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="T2">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E32B68E-D42B-4786-BFE5-4B2187F4D12D}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13439,7 +13963,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13527,7 +14051,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="46" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13538,7 +14062,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13605,7 +14129,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="45" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13990,7 +14514,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="44" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>